<commit_message>
finish send post function and save & delete button
</commit_message>
<xml_diff>
--- a/doc/init_data.xlsx
+++ b/doc/init_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66">
   <si>
     <t>用电设备名称</t>
   </si>
@@ -187,7 +187,7 @@
     <t>空调风机</t>
   </si>
   <si>
-    <t>空调水泵</t>
+    <t>空调水泵1</t>
   </si>
   <si>
     <t>冷藏压缩机</t>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>空调</t>
+  </si>
+  <si>
+    <t>空调水泵2</t>
   </si>
   <si>
     <t>通风风机</t>
@@ -216,116 +219,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -345,9 +250,83 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,31 +340,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -404,7 +393,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,7 +405,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,7 +423,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,25 +483,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,13 +507,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,91 +561,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,6 +590,45 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -612,26 +640,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,21 +659,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -675,174 +668,170 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
     </xf>
@@ -856,7 +845,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
@@ -865,10 +854,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -1192,8 +1178,8 @@
   <sheetPr/>
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1371,7 +1357,7 @@
       <c r="D3" s="4">
         <v>16</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="1">
         <v>0.8</v>
       </c>
       <c r="F3" s="1">
@@ -1439,7 +1425,7 @@
       <c r="D4" s="5">
         <v>6</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="1">
         <v>0.79</v>
       </c>
       <c r="F4" s="1">
@@ -1507,7 +1493,7 @@
       <c r="D5" s="4">
         <v>15</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="1">
         <v>0.89</v>
       </c>
       <c r="F5" s="1">
@@ -1575,7 +1561,7 @@
       <c r="D6" s="5">
         <v>4.5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1">
@@ -1643,7 +1629,7 @@
       <c r="D7" s="5">
         <v>5.5</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="1">
         <v>0.86</v>
       </c>
       <c r="F7" s="1">
@@ -1711,7 +1697,7 @@
       <c r="D8" s="5">
         <v>6</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1">
@@ -1779,7 +1765,7 @@
       <c r="D9" s="7">
         <v>11</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="1">
         <v>0.88</v>
       </c>
       <c r="F9" s="1">
@@ -1847,7 +1833,7 @@
       <c r="D10" s="5">
         <v>5.5</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="1">
         <v>0.86</v>
       </c>
       <c r="F10" s="1">
@@ -1915,7 +1901,7 @@
       <c r="D11" s="5">
         <v>5.5</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="1">
         <v>0.86</v>
       </c>
       <c r="F11" s="1">
@@ -1983,7 +1969,7 @@
       <c r="D12" s="4">
         <v>45</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="1">
         <v>0.92</v>
       </c>
       <c r="F12" s="1">
@@ -2051,7 +2037,7 @@
       <c r="D13" s="5">
         <v>3.3</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="1">
@@ -2119,7 +2105,7 @@
       <c r="D14" s="5">
         <v>1.5</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="1">
         <v>0.79</v>
       </c>
       <c r="F14" s="1">
@@ -2187,7 +2173,7 @@
       <c r="D15" s="5">
         <v>1.5</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="1">
         <v>0.79</v>
       </c>
       <c r="F15" s="1">
@@ -2255,7 +2241,7 @@
       <c r="D16" s="5">
         <v>5.5</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="1">
         <v>0.86</v>
       </c>
       <c r="F16" s="1">
@@ -2323,7 +2309,7 @@
       <c r="D17" s="5">
         <v>7.5</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="1">
         <v>0.87</v>
       </c>
       <c r="F17" s="1">
@@ -2391,7 +2377,7 @@
       <c r="D18" s="5">
         <v>7.5</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="1">
         <v>0.87</v>
       </c>
       <c r="F18" s="1">
@@ -2459,7 +2445,7 @@
       <c r="D19" s="5">
         <v>1.75</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -2527,7 +2513,7 @@
       <c r="D20" s="5">
         <v>4</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20" s="1">
@@ -2595,7 +2581,7 @@
       <c r="D21" s="5">
         <v>2.25</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" s="1">
@@ -2663,7 +2649,7 @@
       <c r="D22" s="5">
         <v>3</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="1">
         <v>0.84</v>
       </c>
       <c r="F22" s="1">
@@ -2731,7 +2717,7 @@
       <c r="D23" s="5">
         <v>3</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="1">
         <v>0.84</v>
       </c>
       <c r="F23" s="1">
@@ -2799,7 +2785,7 @@
       <c r="D24" s="5">
         <v>2.2</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="1">
         <v>0.8</v>
       </c>
       <c r="F24" s="1">
@@ -2867,7 +2853,7 @@
       <c r="D25" s="4">
         <v>12</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" s="1">
@@ -2935,7 +2921,7 @@
       <c r="D26" s="5">
         <v>0.6</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="1">
         <v>0.7</v>
       </c>
       <c r="F26" s="1">
@@ -3003,7 +2989,7 @@
       <c r="D27" s="5">
         <v>0.5</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="1">
         <v>0.7</v>
       </c>
       <c r="F27" s="1">
@@ -3071,7 +3057,7 @@
       <c r="D28" s="4">
         <v>11</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="1">
         <v>0.88</v>
       </c>
       <c r="F28" s="1">
@@ -3139,7 +3125,7 @@
       <c r="D29" s="5">
         <v>2.2</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="1">
         <v>0.84</v>
       </c>
       <c r="F29" s="1">
@@ -3207,7 +3193,7 @@
       <c r="D30" s="5">
         <v>4</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="1">
         <v>1</v>
       </c>
       <c r="F30" s="1">
@@ -3275,55 +3261,55 @@
       <c r="D31" s="7">
         <v>18.5</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="1">
         <v>0.91</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
       </c>
-      <c r="G31" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="H31" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="I31" s="9">
+      <c r="G31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="I31" s="8">
         <v>1</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K31" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="L31" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="M31" s="9">
+      <c r="K31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="L31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="M31" s="8">
         <v>1</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O31" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="P31" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="Q31" s="9">
+      <c r="O31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="P31" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="Q31" s="8">
         <v>1</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S31" s="9">
+      <c r="S31" s="8">
         <v>0.6</v>
       </c>
-      <c r="T31" s="9">
+      <c r="T31" s="8">
         <v>0.6</v>
       </c>
-      <c r="U31" s="9">
+      <c r="U31" s="8">
         <v>1</v>
       </c>
       <c r="V31" s="1" t="s">
@@ -3343,7 +3329,7 @@
       <c r="D32" s="5">
         <v>7.5</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="1">
         <v>0.86</v>
       </c>
       <c r="F32" s="1">
@@ -3411,7 +3397,7 @@
       <c r="D33" s="5">
         <v>4</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="1">
         <v>0.86</v>
       </c>
       <c r="F33" s="1">
@@ -3479,7 +3465,7 @@
       <c r="D34" s="5">
         <v>3.7</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="1">
@@ -3547,7 +3533,7 @@
       <c r="D35" s="5">
         <v>0.18</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
@@ -3615,7 +3601,7 @@
       <c r="D36" s="4">
         <v>18.3</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="1">
@@ -3672,7 +3658,7 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B37" s="6">
         <v>1</v>
@@ -3683,7 +3669,7 @@
       <c r="D37" s="5">
         <v>2.2</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="1">
         <v>0.83</v>
       </c>
       <c r="F37" s="1">
@@ -3740,7 +3726,7 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
@@ -3751,7 +3737,7 @@
       <c r="D38" s="4">
         <v>12</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="1">
         <v>0</v>
       </c>
       <c r="F38" s="1">
@@ -3808,7 +3794,7 @@
     </row>
     <row r="39" spans="1:22">
       <c r="A39" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -3819,43 +3805,43 @@
       <c r="D39" s="5">
         <v>0</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="1">
         <v>0</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
       </c>
-      <c r="G39" s="9">
-        <v>1</v>
-      </c>
-      <c r="H39" s="9">
-        <v>1</v>
-      </c>
-      <c r="I39" s="9">
+      <c r="G39" s="8">
+        <v>1</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1</v>
+      </c>
+      <c r="I39" s="8">
         <v>0.8</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="9">
-        <v>1</v>
-      </c>
-      <c r="L39" s="9">
-        <v>1</v>
-      </c>
-      <c r="M39" s="9">
+      <c r="K39" s="8">
+        <v>1</v>
+      </c>
+      <c r="L39" s="8">
+        <v>1</v>
+      </c>
+      <c r="M39" s="8">
         <v>0.8</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O39" s="9">
-        <v>1</v>
-      </c>
-      <c r="P39" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="9">
+      <c r="O39" s="8">
+        <v>1</v>
+      </c>
+      <c r="P39" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="8">
         <v>0.8</v>
       </c>
       <c r="R39" s="1" t="s">
@@ -3876,7 +3862,7 @@
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -3887,43 +3873,43 @@
       <c r="D40" s="5">
         <v>0</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
       </c>
-      <c r="G40" s="9">
-        <v>1</v>
-      </c>
-      <c r="H40" s="9">
-        <v>1</v>
-      </c>
-      <c r="I40" s="9">
+      <c r="G40" s="8">
+        <v>1</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8">
         <v>0.8</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="9">
-        <v>1</v>
-      </c>
-      <c r="L40" s="9">
-        <v>1</v>
-      </c>
-      <c r="M40" s="9">
+      <c r="K40" s="8">
+        <v>1</v>
+      </c>
+      <c r="L40" s="8">
+        <v>1</v>
+      </c>
+      <c r="M40" s="8">
         <v>1</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O40" s="9">
-        <v>1</v>
-      </c>
-      <c r="P40" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="9">
+      <c r="O40" s="8">
+        <v>1</v>
+      </c>
+      <c r="P40" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="8">
         <v>1</v>
       </c>
       <c r="R40" s="1" t="s">
@@ -3944,7 +3930,7 @@
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -3955,55 +3941,55 @@
       <c r="D41" s="5">
         <v>0</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="1">
         <v>0</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
       </c>
-      <c r="G41" s="9">
-        <v>1</v>
-      </c>
-      <c r="H41" s="9">
-        <v>1</v>
-      </c>
-      <c r="I41" s="9">
+      <c r="G41" s="8">
+        <v>1</v>
+      </c>
+      <c r="H41" s="8">
+        <v>1</v>
+      </c>
+      <c r="I41" s="8">
         <v>0.5</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K41" s="9">
-        <v>1</v>
-      </c>
-      <c r="L41" s="9">
-        <v>1</v>
-      </c>
-      <c r="M41" s="9">
+      <c r="K41" s="8">
+        <v>1</v>
+      </c>
+      <c r="L41" s="8">
+        <v>1</v>
+      </c>
+      <c r="M41" s="8">
         <v>0.5</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O41" s="9">
-        <v>1</v>
-      </c>
-      <c r="P41" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="9">
+      <c r="O41" s="8">
+        <v>1</v>
+      </c>
+      <c r="P41" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="8">
         <v>0.5</v>
       </c>
       <c r="R41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S41" s="9">
-        <v>1</v>
-      </c>
-      <c r="T41" s="9">
-        <v>1</v>
-      </c>
-      <c r="U41" s="9">
+      <c r="S41" s="8">
+        <v>1</v>
+      </c>
+      <c r="T41" s="8">
+        <v>1</v>
+      </c>
+      <c r="U41" s="8">
         <v>0.5</v>
       </c>
       <c r="V41" s="1" t="s">

</xml_diff>

<commit_message>
results page almost finished
</commit_message>
<xml_diff>
--- a/doc/init_data.xlsx
+++ b/doc/init_data.xlsx
@@ -219,11 +219,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -231,6 +231,36 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -243,6 +273,66 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -250,7 +340,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,10 +355,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,99 +370,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,7 +387,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,43 +531,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,7 +549,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,115 +561,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,60 +578,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -652,11 +598,33 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,10 +638,42 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -683,148 +683,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -845,7 +845,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
@@ -854,7 +854,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -1178,8 +1178,8 @@
   <sheetPr/>
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1293,7 +1293,7 @@
         <v>0.84</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="5">
         <v>0.5</v>
@@ -1332,13 +1332,13 @@
         <v>23</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>24</v>
@@ -1361,16 +1361,16 @@
         <v>0.8</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>24</v>
@@ -1388,25 +1388,25 @@
         <v>23</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>24</v>
@@ -1429,16 +1429,16 @@
         <v>0.79</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>24</v>
@@ -1456,25 +1456,25 @@
         <v>23</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>24</v>
@@ -1497,28 +1497,28 @@
         <v>0.89</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>24</v>
@@ -1536,13 +1536,13 @@
         <v>28</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>24</v>
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -1633,28 +1633,28 @@
         <v>0.86</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>24</v>
@@ -1672,13 +1672,13 @@
         <v>28</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>24</v>
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1769,52 +1769,52 @@
         <v>0.88</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="S9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>24</v>
@@ -1837,52 +1837,52 @@
         <v>0.86</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="O10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="S10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>24</v>
@@ -1905,7 +1905,7 @@
         <v>0.86</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="5">
         <v>0.8</v>
@@ -1944,13 +1944,13 @@
         <v>23</v>
       </c>
       <c r="S11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>24</v>
@@ -1973,28 +1973,28 @@
         <v>0.92</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>24</v>
@@ -2012,13 +2012,13 @@
         <v>28</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>24</v>
@@ -2038,10 +2038,10 @@
         <v>3.3</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="5">
         <v>0.8</v>
@@ -2109,7 +2109,7 @@
         <v>0.79</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
         <v>0.8</v>
@@ -2148,13 +2148,13 @@
         <v>30</v>
       </c>
       <c r="S14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>24</v>
@@ -2177,7 +2177,7 @@
         <v>0.79</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="5">
         <v>0.8</v>
@@ -2216,13 +2216,13 @@
         <v>30</v>
       </c>
       <c r="S15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>24</v>
@@ -2245,7 +2245,7 @@
         <v>0.86</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <v>0.8</v>
@@ -2313,7 +2313,7 @@
         <v>0.87</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="5">
         <v>0.8</v>
@@ -2381,7 +2381,7 @@
         <v>0.87</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="5">
         <v>0.8</v>
@@ -2446,10 +2446,10 @@
         <v>1.75</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="5">
         <v>0.8</v>
@@ -2514,10 +2514,10 @@
         <v>4</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="5">
         <v>0.8</v>
@@ -2582,10 +2582,10 @@
         <v>2.25</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5">
         <v>1</v>
@@ -2653,7 +2653,7 @@
         <v>0.84</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
         <v>1</v>
@@ -2721,7 +2721,7 @@
         <v>0.84</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5">
         <v>1</v>
@@ -2760,13 +2760,13 @@
         <v>23</v>
       </c>
       <c r="S23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="1" t="s">
         <v>24</v>
@@ -2789,7 +2789,7 @@
         <v>0.8</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="5">
         <v>0.8</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="5">
         <v>1</v>
@@ -2925,7 +2925,7 @@
         <v>0.7</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -2993,7 +2993,7 @@
         <v>0.7</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="5">
         <v>1</v>
@@ -3061,7 +3061,7 @@
         <v>0.88</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="5">
         <v>0.4</v>
@@ -3100,13 +3100,13 @@
         <v>23</v>
       </c>
       <c r="S28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="1" t="s">
         <v>24</v>
@@ -3129,7 +3129,7 @@
         <v>0.84</v>
       </c>
       <c r="F29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="5">
         <v>0.8</v>
@@ -3197,7 +3197,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="5">
         <v>0.8</v>
@@ -3236,13 +3236,13 @@
         <v>23</v>
       </c>
       <c r="S30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30" s="1" t="s">
         <v>24</v>
@@ -3265,7 +3265,7 @@
         <v>0.91</v>
       </c>
       <c r="F31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="8">
         <v>0.8</v>
@@ -3333,7 +3333,7 @@
         <v>0.86</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="5">
         <v>1</v>
@@ -3401,7 +3401,7 @@
         <v>0.86</v>
       </c>
       <c r="F33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="5">
         <v>0.8</v>
@@ -3466,10 +3466,10 @@
         <v>3.7</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="5">
         <v>0.8</v>
@@ -3534,10 +3534,10 @@
         <v>0.18</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="5">
         <v>1</v>
@@ -3602,10 +3602,10 @@
         <v>18.3</v>
       </c>
       <c r="E36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="5">
         <v>0.8</v>
@@ -3673,7 +3673,7 @@
         <v>0.83</v>
       </c>
       <c r="F37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="5">
         <v>0.8</v>
@@ -3738,10 +3738,10 @@
         <v>12</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="5">
         <v>1</v>
@@ -3806,10 +3806,10 @@
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="8">
         <v>1</v>
@@ -3874,10 +3874,10 @@
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="8">
         <v>1</v>
@@ -3942,10 +3942,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="8">
         <v>1</v>

</xml_diff>